<commit_message>
Updated Product Backlog for Sprint 2
</commit_message>
<xml_diff>
--- a/Product_Backlog/ProductBacklog.xlsx
+++ b/Product_Backlog/ProductBacklog.xlsx
@@ -23,6 +23,12 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="73">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -99,9 +105,6 @@
     <t>FINISH</t>
   </si>
   <si>
-    <t>C. Jones</t>
-  </si>
-  <si>
     <t>AGILE PRODUCT BACKLOG TEMPLATE</t>
   </si>
   <si>
@@ -189,12 +192,6 @@
     <t>1. Search the database with the input entered by the user.</t>
   </si>
   <si>
-    <t>2. Implement price filter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Display the result received back to the user. </t>
-  </si>
-  <si>
     <t>As a website visitor, I want to see the list of hospitals based on the distance entered in the search box</t>
   </si>
   <si>
@@ -238,6 +235,27 @@
   </si>
   <si>
     <t xml:space="preserve"> " "</t>
+  </si>
+  <si>
+    <t>Henry + Topu + Arnav</t>
+  </si>
+  <si>
+    <t>Anthony + Afzal + Matthew</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Henry + Topu</t>
+  </si>
+  <si>
+    <t>1. Implement price filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Display the result received back to the user. </t>
   </si>
 </sst>
 </file>
@@ -775,11 +793,11 @@
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI70"/>
+  <dimension ref="B1:AI69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -787,8 +805,7 @@
     <col min="1" max="1" width="3.25" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="4" customWidth="1"/>
     <col min="3" max="5" width="33.25" style="4" customWidth="1"/>
-    <col min="6" max="7" width="10.75" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
+    <col min="6" max="8" width="11.5" style="4" customWidth="1"/>
     <col min="9" max="9" width="13.75" style="4" customWidth="1"/>
     <col min="10" max="10" width="15.25" style="4" customWidth="1"/>
     <col min="11" max="11" width="16.75" style="4" customWidth="1"/>
@@ -802,7 +819,7 @@
   <sheetData>
     <row r="1" spans="2:35" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -903,36 +920,35 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="F3" s="6">
-        <v>44747</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>43857</v>
+      </c>
+      <c r="G3" s="6">
+        <v>43858</v>
+      </c>
       <c r="H3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="5">
-        <f>SUM(L4:L6)</f>
-        <v>24</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="L3" s="5"/>
       <c r="M3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="3"/>
       <c r="P3"/>
@@ -959,41 +975,39 @@
     <row r="4" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="F4" s="8">
-        <v>44747</v>
+        <v>43857</v>
       </c>
       <c r="G4" s="8">
-        <v>44747</v>
+        <v>43858</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="7">
-        <v>8</v>
-      </c>
+      <c r="L4" s="7"/>
       <c r="M4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="11"/>
@@ -1019,35 +1033,33 @@
     <row r="5" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="F5" s="8">
-        <v>44748</v>
+        <v>43857</v>
       </c>
       <c r="G5" s="8">
-        <v>44749</v>
+        <v>43858</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="7">
-        <v>16</v>
-      </c>
+      <c r="L5" s="7"/>
       <c r="M5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1083,35 +1095,33 @@
     <row r="6" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="F6" s="8">
-        <v>44750</v>
+        <v>43857</v>
       </c>
       <c r="G6" s="8">
-        <v>44751</v>
+        <v>43858</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="7">
-        <v>0</v>
-      </c>
+      <c r="L6" s="7"/>
       <c r="M6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1149,20 +1159,36 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="6">
+        <v>43857</v>
+      </c>
+      <c r="G7" s="6">
+        <v>43860</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12" t="s">
@@ -1193,20 +1219,36 @@
     <row r="8" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="8">
+        <v>43857</v>
+      </c>
+      <c r="G8" s="8">
+        <v>43860</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="M8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -1230,20 +1272,36 @@
     <row r="9" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="8">
+        <v>43857</v>
+      </c>
+      <c r="G9" s="8">
+        <v>43860</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1308,20 +1366,36 @@
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="6">
+        <v>43858</v>
+      </c>
+      <c r="G11" s="6">
+        <v>43858</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -1348,20 +1422,36 @@
     <row r="12" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="8">
+        <v>43858</v>
+      </c>
+      <c r="G12" s="8">
+        <v>43858</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="M12" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -1388,20 +1478,36 @@
     <row r="13" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="8">
+        <v>43858</v>
+      </c>
+      <c r="G13" s="8">
+        <v>43858</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="M13" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -1466,20 +1572,34 @@
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
+      <c r="E15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="6">
+        <v>43858</v>
+      </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -1506,20 +1626,34 @@
     <row r="16" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="8">
+        <v>43858</v>
+      </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="M16" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1546,20 +1680,34 @@
     <row r="17" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="8">
+        <v>43858</v>
+      </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="M17" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -1624,20 +1772,34 @@
         <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6">
+        <v>43858</v>
+      </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="M19" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -1664,20 +1826,34 @@
     <row r="20" spans="2:35" ht="67.5" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="8">
+        <v>43858</v>
+      </c>
       <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="M20" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -1704,20 +1880,34 @@
     <row r="21" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="8">
+        <v>43858</v>
+      </c>
       <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="M21" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -1782,20 +1972,34 @@
         <v>6</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
+      <c r="E23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="6">
+        <v>43857</v>
+      </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="M23" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -1932,20 +2136,34 @@
         <v>7</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
+      <c r="E27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="6">
+        <v>43865</v>
+      </c>
       <c r="G27" s="6"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="M27" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -1972,20 +2190,34 @@
     <row r="28" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="8">
+        <v>43865</v>
+      </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
+      <c r="H28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="M28" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -2012,20 +2244,34 @@
     <row r="29" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="8">
+        <v>43865</v>
+      </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="H29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="M29" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -2052,20 +2298,32 @@
     <row r="30" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
+      <c r="H30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
+      <c r="M30" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -2094,20 +2352,32 @@
         <v>8</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -2134,20 +2404,32 @@
     <row r="32" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
+      <c r="H32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
+      <c r="M32" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
@@ -2174,20 +2456,32 @@
     <row r="33" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
+      <c r="M33" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -2214,20 +2508,32 @@
     <row r="34" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
+      <c r="H34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
+      <c r="M34" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -2256,20 +2562,32 @@
         <v>9</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+      <c r="H35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -2293,23 +2611,35 @@
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
     </row>
-    <row r="36" spans="2:35" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
+      <c r="H36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
+      <c r="M36" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -2333,23 +2663,35 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
+      <c r="H37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
+      <c r="M37" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -2373,23 +2715,37 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
     </row>
-    <row r="38" spans="2:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
+    <row r="38" spans="2:35" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
+        <v>10</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -2413,25 +2769,35 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="2:35" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="5">
-        <v>10</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
+    <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -2458,20 +2824,32 @@
     <row r="40" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
+      <c r="M40" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -2498,20 +2876,32 @@
     <row r="41" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
+      <c r="H41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
+      <c r="M41" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -2535,23 +2925,37 @@
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
     </row>
-    <row r="42" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
+    <row r="42" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="5">
+        <v>11</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
@@ -2575,25 +2979,35 @@
       <c r="AH42" s="3"/>
       <c r="AI42" s="3"/>
     </row>
-    <row r="43" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="5">
-        <v>11</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
+    <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
@@ -2620,20 +3034,32 @@
     <row r="44" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
+      <c r="H44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
+      <c r="M44" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -2659,12 +3085,8 @@
     </row>
     <row r="45" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
-      <c r="C45" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2697,19 +3119,37 @@
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
     </row>
-    <row r="46" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
+    <row r="46" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="5">
+        <v>12</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -2734,24 +3174,34 @@
       <c r="AI46" s="3"/>
     </row>
     <row r="47" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="5">
-        <v>12</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -2775,23 +3225,35 @@
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
     </row>
-    <row r="48" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="7" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
+      <c r="H48" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
+      <c r="M48" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
@@ -2817,12 +3279,8 @@
     </row>
     <row r="49" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -2856,18 +3314,36 @@
       <c r="AI49" s="3"/>
     </row>
     <row r="50" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
+      <c r="B50" s="5">
+        <v>13</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
@@ -2891,25 +3367,39 @@
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
     </row>
-    <row r="51" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="5">
-        <v>13</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
+    <row r="51" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" s="8">
+        <v>43864</v>
+      </c>
+      <c r="G51" s="8">
+        <v>43865</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
@@ -2933,14 +3423,10 @@
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
     </row>
-    <row r="52" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
-      <c r="C52" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -3009,19 +3495,37 @@
       <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
     </row>
-    <row r="54" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
+    <row r="54" spans="2:35" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
+        <v>14</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
@@ -3045,25 +3549,35 @@
       <c r="AH54" s="3"/>
       <c r="AI54" s="3"/>
     </row>
-    <row r="55" spans="2:35" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="5">
-        <v>14</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
+    <row r="55" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
@@ -3087,14 +3601,10 @@
       <c r="AH55" s="3"/>
       <c r="AI55" s="3"/>
     </row>
-    <row r="56" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
-      <c r="C56" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
@@ -3163,19 +3673,37 @@
       <c r="AH57" s="3"/>
       <c r="AI57" s="3"/>
     </row>
-    <row r="58" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
+    <row r="58" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
+        <v>15</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
@@ -3200,24 +3728,34 @@
       <c r="AI58" s="3"/>
     </row>
     <row r="59" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="5">
-        <v>15</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
@@ -3241,14 +3779,10 @@
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
     </row>
-    <row r="60" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
-      <c r="C60" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
@@ -3317,61 +3851,51 @@
       <c r="AH61" s="3"/>
       <c r="AI61" s="3"/>
     </row>
-    <row r="62" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="7"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-      <c r="Q62" s="3"/>
-      <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
-      <c r="W62" s="3"/>
-      <c r="X62" s="3"/>
-      <c r="Y62" s="3"/>
-      <c r="Z62" s="3"/>
-      <c r="AA62" s="3"/>
-      <c r="AB62" s="3"/>
-      <c r="AC62" s="3"/>
-      <c r="AD62" s="3"/>
-      <c r="AE62" s="3"/>
-      <c r="AF62" s="3"/>
-      <c r="AG62" s="3"/>
-      <c r="AH62" s="3"/>
-      <c r="AI62" s="3"/>
-    </row>
-    <row r="63" spans="2:35" ht="27" x14ac:dyDescent="0.25">
-      <c r="B63" s="5">
+    <row r="62" spans="2:35" ht="27" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
         <v>16</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="C62" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
     </row>
     <row r="64" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
@@ -3401,39 +3925,51 @@
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-    </row>
-    <row r="67" spans="2:13" ht="54" x14ac:dyDescent="0.25">
-      <c r="B67" s="5">
+    <row r="66" spans="2:13" ht="54" x14ac:dyDescent="0.25">
+      <c r="B66" s="5">
         <v>17</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
+      <c r="C66" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
     </row>
     <row r="68" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
@@ -3463,32 +3999,18 @@
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O6">
       <formula1>$A$6:$A$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I70 M3:M70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M69 H3:I69">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J69">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K69">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -3522,7 +4044,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Version of Product Backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/ProductBacklog.xlsx
+++ b/Product_Backlog/ProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAC6FD-A11C-4314-B129-1682DFD353F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC0917D-E809-4FC9-BF49-5333E2B92D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -344,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -413,12 +413,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -455,6 +498,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -803,28 +861,28 @@
   <dimension ref="B1:AI69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="4" customWidth="1"/>
-    <col min="3" max="5" width="33.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="4" customWidth="1"/>
+    <col min="3" max="5" width="33.19921875" style="4" customWidth="1"/>
     <col min="6" max="8" width="11.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.75" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.25" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.75" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.75" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.25" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.25" style="4" customWidth="1"/>
-    <col min="15" max="17" width="17.75" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.25" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="10.75" style="4"/>
+    <col min="9" max="9" width="13.69921875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.19921875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.69921875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.69921875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.19921875" style="4" customWidth="1"/>
+    <col min="15" max="17" width="17.69921875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.19921875" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="10.69921875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:35" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>22</v>
       </c>
@@ -862,7 +920,7 @@
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
-    <row r="2" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -922,7 +980,7 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -981,7 +1039,7 @@
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
     </row>
-    <row r="4" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
         <v>27</v>
@@ -1010,7 +1068,9 @@
       <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="7">
+        <v>2</v>
+      </c>
       <c r="M4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1099,7 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
     </row>
-    <row r="5" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
         <v>29</v>
@@ -1068,7 +1128,9 @@
       <c r="K5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
       <c r="M5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1101,7 +1163,7 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
         <v>30</v>
@@ -1130,7 +1192,9 @@
       <c r="K6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="7"/>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
       <c r="M6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1163,7 +1227,7 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>2</v>
       </c>
@@ -1227,7 +1291,7 @@
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>31</v>
@@ -1282,7 +1346,7 @@
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>32</v>
@@ -1340,7 +1404,7 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
     </row>
-    <row r="10" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1376,7 +1440,7 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -1436,7 +1500,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
         <v>35</v>
@@ -1494,7 +1558,7 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
         <v>36</v>
@@ -1552,7 +1616,7 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1588,7 +1652,7 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>4</v>
       </c>
@@ -1611,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>5</v>
@@ -1648,7 +1712,7 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
     </row>
-    <row r="16" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
         <v>37</v>
@@ -1663,18 +1727,18 @@
         <v>43858</v>
       </c>
       <c r="G16" s="8">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="7">
@@ -1706,7 +1770,7 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
         <v>36</v>
@@ -1727,12 +1791,12 @@
         <v>3</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L17" s="7">
@@ -1764,7 +1828,7 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1800,7 +1864,7 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>5</v>
       </c>
@@ -1816,14 +1880,14 @@
       <c r="F19" s="6">
         <v>43858</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="6">
         <v>43867</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>6</v>
@@ -1860,7 +1924,7 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="2:35" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" ht="79.2" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
         <v>39</v>
@@ -1881,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>6</v>
@@ -1918,7 +1982,7 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
         <v>36</v>
@@ -1939,7 +2003,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>6</v>
@@ -1976,7 +2040,7 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -2012,7 +2076,7 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="2:35" ht="54" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" ht="52.8" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -2035,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>5</v>
@@ -2072,7 +2136,7 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -2108,7 +2172,7 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -2144,7 +2208,7 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2180,7 +2244,7 @@
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>7</v>
       </c>
@@ -2203,7 +2267,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>5</v>
@@ -2240,7 +2304,7 @@
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>43</v>
@@ -2254,19 +2318,19 @@
       <c r="F28" s="8">
         <v>43865</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="19">
         <v>43866</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>3</v>
+      <c r="I28" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="K28" s="15" t="s">
         <v>7</v>
       </c>
       <c r="L28" s="7">
@@ -2298,7 +2362,7 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
         <v>42</v>
@@ -2312,19 +2376,19 @@
       <c r="F29" s="8">
         <v>43865</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="19">
         <v>43866</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>3</v>
+      <c r="I29" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="17" t="s">
         <v>7</v>
       </c>
       <c r="L29" s="7">
@@ -2356,7 +2420,7 @@
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="2:35" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:35" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>44</v>
@@ -2371,18 +2435,18 @@
         <v>43865</v>
       </c>
       <c r="G30" s="8">
-        <v>43865</v>
+        <v>43866</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>3</v>
+      <c r="I30" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="K30" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L30" s="7">
@@ -2414,7 +2478,7 @@
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
     </row>
-    <row r="31" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5">
         <v>8</v>
       </c>
@@ -2437,7 +2501,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>5</v>
@@ -2474,7 +2538,7 @@
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
     </row>
-    <row r="32" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>46</v>
@@ -2494,8 +2558,8 @@
       <c r="H32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="7" t="s">
-        <v>3</v>
+      <c r="I32" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>5</v>
@@ -2532,7 +2596,7 @@
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
     </row>
-    <row r="33" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>47</v>
@@ -2552,7 +2616,7 @@
       <c r="H33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I33" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J33" s="7" t="s">
@@ -2590,7 +2654,7 @@
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
-    <row r="34" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>48</v>
@@ -2610,8 +2674,8 @@
       <c r="H34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="7" t="s">
-        <v>3</v>
+      <c r="I34" s="17" t="s">
+        <v>2</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>5</v>
@@ -2648,7 +2712,7 @@
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
     </row>
-    <row r="35" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:35" ht="52.8" x14ac:dyDescent="0.3">
       <c r="B35" s="5">
         <v>9</v>
       </c>
@@ -2671,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>6</v>
@@ -2708,7 +2772,7 @@
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
     </row>
-    <row r="36" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>68</v>
@@ -2728,13 +2792,13 @@
       <c r="H36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I36" s="7" t="s">
-        <v>3</v>
+      <c r="I36" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L36" s="7">
@@ -2766,7 +2830,7 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="2:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>69</v>
@@ -2786,13 +2850,13 @@
       <c r="H37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="7" t="s">
-        <v>3</v>
+      <c r="I37" s="17" t="s">
+        <v>2</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L37" s="7">
@@ -2824,7 +2888,7 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
     </row>
-    <row r="38" spans="2:35" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:35" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="5">
         <v>10</v>
       </c>
@@ -2847,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>6</v>
@@ -2884,7 +2948,7 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
         <v>73</v>
@@ -2904,13 +2968,13 @@
       <c r="H39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>3</v>
+      <c r="I39" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K39" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L39" s="7">
@@ -2942,7 +3006,7 @@
       <c r="AH39" s="3"/>
       <c r="AI39" s="3"/>
     </row>
-    <row r="40" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
         <v>74</v>
@@ -2962,13 +3026,13 @@
       <c r="H40" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I40" s="7" t="s">
-        <v>3</v>
+      <c r="I40" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="J40" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="K40" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L40" s="7">
@@ -3000,7 +3064,7 @@
       <c r="AH40" s="3"/>
       <c r="AI40" s="3"/>
     </row>
-    <row r="41" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B41" s="5">
         <v>11</v>
       </c>
@@ -3060,7 +3124,7 @@
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
     </row>
-    <row r="42" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
         <v>51</v>
@@ -3080,7 +3144,7 @@
       <c r="H42" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" s="18" t="s">
         <v>2</v>
       </c>
       <c r="J42" s="7" t="s">
@@ -3118,7 +3182,7 @@
       <c r="AH42" s="3"/>
       <c r="AI42" s="3"/>
     </row>
-    <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
         <v>36</v>
@@ -3138,7 +3202,7 @@
       <c r="H43" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" s="18" t="s">
         <v>2</v>
       </c>
       <c r="J43" s="7" t="s">
@@ -3176,7 +3240,7 @@
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
     </row>
-    <row r="44" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -3212,7 +3276,7 @@
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
     </row>
-    <row r="45" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B45" s="5">
         <v>12</v>
       </c>
@@ -3272,7 +3336,7 @@
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
     </row>
-    <row r="46" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="7" t="s">
         <v>52</v>
@@ -3330,7 +3394,7 @@
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
     </row>
-    <row r="47" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7" t="s">
         <v>36</v>
@@ -3388,7 +3452,7 @@
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
     </row>
-    <row r="48" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -3424,7 +3488,7 @@
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
     </row>
-    <row r="49" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="5">
         <v>13</v>
       </c>
@@ -3484,7 +3548,7 @@
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
     </row>
-    <row r="50" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="7" t="s">
         <v>54</v>
@@ -3542,7 +3606,7 @@
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
     </row>
-    <row r="51" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -3578,7 +3642,7 @@
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
     </row>
-    <row r="52" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -3614,7 +3678,7 @@
       <c r="AH52" s="3"/>
       <c r="AI52" s="3"/>
     </row>
-    <row r="53" spans="2:35" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:35" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -3637,7 +3701,7 @@
         <v>2</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>4</v>
@@ -3674,7 +3738,7 @@
       <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
     </row>
-    <row r="54" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="7" t="s">
         <v>56</v>
@@ -3695,7 +3759,7 @@
         <v>3</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J54" s="7" t="s">
         <v>4</v>
@@ -3732,7 +3796,7 @@
       <c r="AH54" s="3"/>
       <c r="AI54" s="3"/>
     </row>
-    <row r="55" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -3768,7 +3832,7 @@
       <c r="AH55" s="3"/>
       <c r="AI55" s="3"/>
     </row>
-    <row r="56" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -3804,7 +3868,7 @@
       <c r="AH56" s="3"/>
       <c r="AI56" s="3"/>
     </row>
-    <row r="57" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B57" s="5">
         <v>15</v>
       </c>
@@ -3864,7 +3928,7 @@
       <c r="AH57" s="3"/>
       <c r="AI57" s="3"/>
     </row>
-    <row r="58" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="7" t="s">
         <v>58</v>
@@ -3922,7 +3986,7 @@
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
     </row>
-    <row r="59" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" s="7" t="s">
         <v>70</v>
@@ -3980,7 +4044,7 @@
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
     </row>
-    <row r="60" spans="2:35" ht="27" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="7" t="s">
         <v>71</v>
@@ -4038,7 +4102,7 @@
       <c r="AH60" s="3"/>
       <c r="AI60" s="3"/>
     </row>
-    <row r="61" spans="2:35" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:35" ht="39.6" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
       <c r="C61" s="7" t="s">
         <v>72</v>
@@ -4096,7 +4160,7 @@
       <c r="AH61" s="3"/>
       <c r="AI61" s="3"/>
     </row>
-    <row r="62" spans="2:35" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:35" ht="26.4" x14ac:dyDescent="0.3">
       <c r="B62" s="5">
         <v>16</v>
       </c>
@@ -4134,7 +4198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -4148,7 +4212,7 @@
       <c r="L63" s="7"/>
       <c r="M63" s="7"/>
     </row>
-    <row r="64" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -4162,7 +4226,7 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -4176,7 +4240,7 @@
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="2:13" ht="54" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" ht="52.8" x14ac:dyDescent="0.3">
       <c r="B66" s="5">
         <v>17</v>
       </c>
@@ -4214,7 +4278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -4228,7 +4292,7 @@
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -4242,7 +4306,7 @@
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -4292,14 +4356,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="13" customWidth="1"/>
-    <col min="2" max="2" width="88.25" style="13" customWidth="1"/>
-    <col min="3" max="16384" width="10.75" style="13"/>
+    <col min="1" max="1" width="3.19921875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="88.19921875" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="10.69921875" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Final Version of Project Backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/ProductBacklog.xlsx
+++ b/Product_Backlog/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC0917D-E809-4FC9-BF49-5333E2B92D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D47932-C50B-4E59-A3CB-6CB8FFEC19CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,8 +22,14 @@
     <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -862,7 +868,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -2492,7 +2498,7 @@
         <v>63</v>
       </c>
       <c r="F31" s="6">
-        <v>43858</v>
+        <v>43866</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>76</v>
@@ -2550,7 +2556,7 @@
         <v>63</v>
       </c>
       <c r="F32" s="8">
-        <v>43858</v>
+        <v>43866</v>
       </c>
       <c r="G32" s="8">
         <v>43866</v>
@@ -2608,7 +2614,7 @@
         <v>63</v>
       </c>
       <c r="F33" s="8">
-        <v>43867</v>
+        <v>43866</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>76</v>
@@ -2666,7 +2672,7 @@
         <v>75</v>
       </c>
       <c r="F34" s="8">
-        <v>43862</v>
+        <v>43867</v>
       </c>
       <c r="G34" s="8">
         <v>43867</v>
@@ -2726,7 +2732,7 @@
         <v>64</v>
       </c>
       <c r="F35" s="6">
-        <v>43862</v>
+        <v>43866</v>
       </c>
       <c r="G35" s="6">
         <v>43866</v>
@@ -2784,7 +2790,7 @@
         <v>64</v>
       </c>
       <c r="F36" s="8">
-        <v>43862</v>
+        <v>43866</v>
       </c>
       <c r="G36" s="8">
         <v>43866</v>
@@ -2842,7 +2848,7 @@
         <v>64</v>
       </c>
       <c r="F37" s="8">
-        <v>43863</v>
+        <v>43866</v>
       </c>
       <c r="G37" s="8">
         <v>43866</v>
@@ -2920,7 +2926,7 @@
         <v>7</v>
       </c>
       <c r="L38" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>2</v>
@@ -3096,7 +3102,7 @@
         <v>7</v>
       </c>
       <c r="L41" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M41" s="5" t="s">
         <v>2</v>
@@ -3308,7 +3314,7 @@
         <v>7</v>
       </c>
       <c r="L45" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>2</v>
@@ -3710,7 +3716,7 @@
         <v>7</v>
       </c>
       <c r="L53" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>2</v>

</xml_diff>